<commit_message>
chore: publish terminology IG 2.0.0-draft
</commit_message>
<xml_diff>
--- a/ig/terminology/CodeSystem-medcom-observation-resultGroup.xlsx
+++ b/ig/terminology/CodeSystem-medcom-observation-resultGroup.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.1</t>
+    <t>2.0.0-draft</t>
   </si>
   <si>
     <t>Name</t>
@@ -42,9 +42,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>MedCom Observation Result Group</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -84,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>The observation result group are intende to be used to sort the individual analyzes.</t>
+    <t>The observation result group are intended to be used to sort the individual analyzes.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -463,129 +460,129 @@
         <v>8</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s" s="2">
         <v>10</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s" s="2">
         <v>12</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>14</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s" s="2">
         <v>16</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>18</v>
-      </c>
-      <c r="B10" t="s" s="2">
-        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>20</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s" s="2">
         <v>22</v>
-      </c>
-      <c r="B12" t="s" s="2">
-        <v>23</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s" s="2">
         <v>26</v>
-      </c>
-      <c r="B15" t="s" s="2">
-        <v>27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s" s="2">
         <v>32</v>
-      </c>
-      <c r="B20" t="s" s="2">
-        <v>33</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s" s="2">
         <v>35</v>
-      </c>
-      <c r="B22" t="s" s="2">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -603,303 +600,303 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>37</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="C1" t="s" s="1">
         <v>38</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="D1" t="s" s="1">
         <v>39</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>40</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>42</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>43</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s" s="2">
         <v>44</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>45</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s" s="2">
         <v>46</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>47</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s" s="2">
         <v>48</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>49</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s" s="2">
         <v>50</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>51</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s" s="2">
         <v>52</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>53</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s" s="2">
         <v>54</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>55</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s" s="2">
         <v>56</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>57</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s" s="2">
         <v>58</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>59</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s" s="2">
         <v>60</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>61</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="C12" t="s" s="2">
         <v>62</v>
-      </c>
-      <c r="C12" t="s" s="2">
-        <v>63</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s" s="2">
         <v>64</v>
-      </c>
-      <c r="C13" t="s" s="2">
-        <v>65</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s" s="2">
         <v>66</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>67</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s" s="2">
         <v>68</v>
-      </c>
-      <c r="C15" t="s" s="2">
-        <v>69</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s" s="2">
         <v>70</v>
-      </c>
-      <c r="C16" t="s" s="2">
-        <v>71</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="C17" t="s" s="2">
         <v>72</v>
-      </c>
-      <c r="C17" t="s" s="2">
-        <v>73</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s" s="2">
         <v>74</v>
-      </c>
-      <c r="C18" t="s" s="2">
-        <v>75</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s" s="2">
         <v>76</v>
-      </c>
-      <c r="C19" t="s" s="2">
-        <v>77</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s" s="2">
         <v>78</v>
-      </c>
-      <c r="C20" t="s" s="2">
-        <v>79</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s" s="2">
         <v>80</v>
-      </c>
-      <c r="C21" t="s" s="2">
-        <v>81</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="C22" t="s" s="2">
         <v>82</v>
-      </c>
-      <c r="C22" t="s" s="2">
-        <v>83</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s" s="2">
         <v>84</v>
-      </c>
-      <c r="C23" t="s" s="2">
-        <v>85</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="C24" t="s" s="2">
-        <v>87</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="C25" t="s" s="2">
-        <v>89</v>
       </c>
       <c r="D25" s="2"/>
     </row>

</xml_diff>